<commit_message>
Pioneer Gliders Calibration and ingest CSV
Updated various Pioneer Calibration files and created associated ingest
CSV files
</commit_message>
<xml_diff>
--- a/CP05MOAS-GL335/Omaha_Cal_Info_CP05MOAS-GL335_00002.xlsx
+++ b/CP05MOAS-GL335/Omaha_Cal_Info_CP05MOAS-GL335_00002.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\Ingest sheets\ingestion-csvs\CP05MOAS-GL335\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="640" windowWidth="23200" windowHeight="8220" tabRatio="377"/>
+    <workbookView xWindow="660" yWindow="645" windowWidth="23205" windowHeight="8220" tabRatio="377"/>
   </bookViews>
   <sheets>
-    <sheet name="Glider" sheetId="1" r:id="rId1"/>
+    <sheet name="Moorings" sheetId="1" r:id="rId1"/>
     <sheet name="Asset_Cal_Info" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Asset_Cal_Info!$A$1:$F$19</definedName>
     <definedName name="_xlnm._FilterDatabase">Asset_Cal_Info!$A$1:$F$19</definedName>
-    <definedName name="_FilterDatabase_0">Glider!#REF!</definedName>
-    <definedName name="_FilterDatabase_0_0">Glider!$A$1:$J$99</definedName>
-    <definedName name="_FilterDatabase_0_0_0">Glider!#REF!</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0">Glider!$A$1:$J$99</definedName>
+    <definedName name="_FilterDatabase_0">Moorings!#REF!</definedName>
+    <definedName name="_FilterDatabase_0_0">Moorings!$A$1:$J$99</definedName>
+    <definedName name="_FilterDatabase_0_0_0">Moorings!#REF!</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0">Moorings!$A$1:$J$99</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$386</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$1</definedName>
@@ -27,10 +32,10 @@
     <definedName name="_FilterDatabase_0_1">Asset_Cal_Info!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_1">Asset_Cal_Info!$A$1:$F$19</definedName>
     <definedName name="_FilterDatabase_1_1">Asset_Cal_Info!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_1_1_1">Glider!$A$1:$J$99</definedName>
+    <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$99</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$386</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -118,24 +123,6 @@
   </si>
   <si>
     <t>No calibration coefficient</t>
-  </si>
-  <si>
-    <t>CP05MOAS-GL001-01-ADCPAM000</t>
-  </si>
-  <si>
-    <t>CP05MOAS-GL001-02-FLORTM000</t>
-  </si>
-  <si>
-    <t>CP05MOAS-GL001-03-CTDGVM000</t>
-  </si>
-  <si>
-    <t>CP05MOAS-GL001-04-DOSTAM000</t>
-  </si>
-  <si>
-    <t>CP05MOAS-GL001-05-PARADM000</t>
-  </si>
-  <si>
-    <t>CP05MOAS-GL001-00-ENG000000</t>
   </si>
   <si>
     <t>AT-31</t>
@@ -162,12 +149,30 @@
   <si>
     <t>EB Line</t>
   </si>
+  <si>
+    <t>CP05MOAS-GL335-01-ADCPAM000</t>
+  </si>
+  <si>
+    <t>CP05MOAS-GL335-02-FLORTM000</t>
+  </si>
+  <si>
+    <t>CP05MOAS-GL335-03-CTDGVM000</t>
+  </si>
+  <si>
+    <t>CP05MOAS-GL335-04-DOSTAM000</t>
+  </si>
+  <si>
+    <t>CP05MOAS-GL335-05-PARADM000</t>
+  </si>
+  <si>
+    <t>CP05MOAS-GL335-00-ENG000000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -255,6 +260,12 @@
       <sz val="12"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -374,7 +385,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -453,6 +464,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -551,6 +565,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -843,23 +860,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:I2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="6" width="17.6640625" customWidth="1"/>
-    <col min="7" max="8" width="19.83203125" customWidth="1"/>
-    <col min="9" max="10" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="10" width="9.7109375" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30">
+    <row r="1" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -894,9 +911,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="6" customFormat="1" ht="15">
+    <row r="2" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2" s="7">
         <v>335</v>
@@ -907,29 +924,39 @@
       <c r="D2" s="25">
         <v>42289</v>
       </c>
-      <c r="E2" s="9"/>
+      <c r="E2" s="9">
+        <v>6.25E-2</v>
+      </c>
       <c r="F2" s="8"/>
       <c r="G2" s="28" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I2" s="29">
         <v>200</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K2" s="30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>30</v>
+      </c>
+      <c r="L2" s="31">
+        <f>((LEFT(G2,(FIND("°",G2,1)-1)))+(MID(G2,(FIND("°",G2,1)+1),(FIND("'",G2,1))-(FIND("°",G2,1)+1))/60))*(IF(RIGHT(G2,1)="N",1,-1))</f>
+        <v>39.833333333333336</v>
+      </c>
+      <c r="M2" s="31">
+        <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="E",1,-1))</f>
+        <v>-70.708333333333329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
@@ -949,21 +976,21 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D18"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" customWidth="1"/>
-    <col min="5" max="5" width="29.5" customWidth="1"/>
-    <col min="6" max="6" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30">
+    <row r="1" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -983,15 +1010,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B2" s="13">
         <v>335</v>
       </c>
       <c r="C2" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2" s="27">
         <v>643111</v>
@@ -1016,15 +1043,15 @@
       <c r="P2" s="16"/>
       <c r="Q2" s="16"/>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B3" s="13">
         <v>335</v>
       </c>
       <c r="C3" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3" s="27">
         <v>643111</v>
@@ -1049,15 +1076,15 @@
       <c r="P3" s="16"/>
       <c r="Q3" s="16"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B4" s="13">
         <v>335</v>
       </c>
       <c r="C4" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D4" s="27">
         <v>643111</v>
@@ -1082,15 +1109,15 @@
       <c r="P4" s="16"/>
       <c r="Q4" s="16"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B5" s="13">
         <v>335</v>
       </c>
       <c r="C5" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D5" s="27">
         <v>643111</v>
@@ -1115,7 +1142,7 @@
       <c r="P5" s="16"/>
       <c r="Q5" s="16"/>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -1134,15 +1161,15 @@
       <c r="P6" s="16"/>
       <c r="Q6" s="16"/>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B7" s="13">
         <v>335</v>
       </c>
       <c r="C7" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D7" s="27">
         <v>2809</v>
@@ -1162,15 +1189,15 @@
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B8" s="13">
         <v>335</v>
       </c>
       <c r="C8" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D8" s="27">
         <v>2809</v>
@@ -1190,15 +1217,15 @@
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B9" s="13">
         <v>335</v>
       </c>
       <c r="C9" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D9" s="27">
         <v>2809</v>
@@ -1218,15 +1245,15 @@
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B10" s="13">
         <v>335</v>
       </c>
       <c r="C10" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D10" s="27">
         <v>2809</v>
@@ -1246,7 +1273,7 @@
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -1260,15 +1287,15 @@
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1">
+    <row r="12" spans="1:17" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B12" s="13">
         <v>335</v>
       </c>
       <c r="C12" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D12" s="27">
         <v>9029</v>
@@ -1284,7 +1311,7 @@
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1298,15 +1325,15 @@
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B14" s="13">
         <v>335</v>
       </c>
       <c r="C14" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D14" s="27">
         <v>105</v>
@@ -1322,7 +1349,7 @@
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1">
+    <row r="15" spans="1:17" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -1336,15 +1363,15 @@
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B16" s="13">
         <v>335</v>
       </c>
       <c r="C16" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D16" s="27">
         <v>50151</v>
@@ -1360,7 +1387,7 @@
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
     </row>
-    <row r="17" spans="1:12" s="4" customFormat="1">
+    <row r="17" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -1374,15 +1401,15 @@
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
     </row>
-    <row r="18" spans="1:12" s="4" customFormat="1">
+    <row r="18" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B18" s="13">
         <v>335</v>
       </c>
       <c r="C18" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D18" s="13">
         <v>335</v>
@@ -1398,7 +1425,7 @@
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
     </row>
-    <row r="19" spans="1:12" s="4" customFormat="1">
+    <row r="19" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>

</xml_diff>